<commit_message>
updata egy conversion factor
</commit_message>
<xml_diff>
--- a/ChinaBalancedSAM/energydata/EGYCONS_IND.xlsx
+++ b/ChinaBalancedSAM/energydata/EGYCONS_IND.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8565" yWindow="285" windowWidth="10710" windowHeight="7140"/>
+    <workbookView xWindow="940" yWindow="140" windowWidth="10710" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="COAL" sheetId="1" r:id="rId1"/>
@@ -2964,13 +2964,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="164" formatCode="0_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2981,7 +2981,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3150,7 +3150,7 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3159,9 +3159,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3204,9 +3201,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3219,7 +3219,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3508,18 +3508,18 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="7" max="8" width="9.75" customWidth="1"/>
+    <col min="2" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="7" max="8" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3542,147 +3542,147 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1">
       <c r="A31" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -3695,762 +3695,763 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.75" customWidth="1"/>
-    <col min="2" max="2" width="48.875" customWidth="1"/>
-    <col min="3" max="3" width="42.625" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="2" max="2" width="48.90625" customWidth="1"/>
+    <col min="3" max="3" width="42.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="21">
+      <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="10" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>0.71430000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <v>0.28570000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <v>0.35720000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="19">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <v>0.97140000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <v>1.4286000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>1.4286000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="17">
         <v>1.4714</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <v>1.4714</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="17">
         <v>1.4571000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="17">
         <v>1.7142999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="17">
         <v>1.5713999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="17">
         <v>1.33</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="18">
         <v>0.59289999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="5" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="17">
         <v>0.17860000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="17">
         <v>0.65710000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="17">
         <v>1.2142999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="17">
         <v>0.55710000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="17">
         <v>0.51429999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="18">
         <v>0.35709999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="17">
         <v>1.1429</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="17">
         <v>1.4286000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="14" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="17">
         <v>3.4099999999999998E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="14" t="s">
+    <row r="31" spans="1:5">
+      <c r="A31" s="9"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="10" t="s">
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="17">
         <v>0.1229</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="10" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="5" t="s">
+      <c r="C33" s="13"/>
+      <c r="D33" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="10" t="s">
+    <row r="34" spans="1:5">
+      <c r="A34" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="5" t="s">
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="17">
         <v>0.64300000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:5">
+      <c r="A36" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="17">
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="10" t="s">
+    <row r="37" spans="1:5">
+      <c r="A37" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="17">
         <v>0.42899999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="10" t="s">
+    <row r="38" spans="1:5">
+      <c r="A38" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="17">
         <v>0.52900000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="10" t="s">
+    <row r="39" spans="1:5">
+      <c r="A39" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="17">
         <v>0.64300000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="10" t="s">
+    <row r="40" spans="1:5">
+      <c r="A40" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="17">
         <v>0.54300000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="10" t="s">
+    <row r="41" spans="1:5">
+      <c r="A41" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="17">
         <v>0.42899999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="10" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="17">
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="10" t="s">
+    <row r="43" spans="1:5">
+      <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E43" s="18">
+      <c r="E43" s="17">
         <v>0.52900000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="10" t="s">
+    <row r="44" spans="1:5">
+      <c r="A44" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E44" s="17">
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="10" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="17">
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="10" t="s">
+    <row r="46" spans="1:5">
+      <c r="A46" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="17">
         <v>0.57099999999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="10" t="s">
+    <row r="47" spans="1:5">
+      <c r="A47" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="17">
         <v>0.71399999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="15"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+    <row r="48" spans="1:5" ht="15" thickBot="1">
+      <c r="A48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>